<commit_message>
Server Updated with UI Service components with localhost:8000, start the node server with 'npm server'
</commit_message>
<xml_diff>
--- a/FinalProject/TestFiles/StudentInfo.xlsx
+++ b/FinalProject/TestFiles/StudentInfo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amritabiswas/Documents/WebProgramming_Workspace/gitRepo/Web_Programming/FinalProject/TestFiles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{134A31E3-7B76-4B48-804A-0C16386AA081}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{298BEC84-616C-4B88-BFDD-252E99891C77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16200" xr2:uid="{8DE653B0-F209-C441-84F9-A72667F02786}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8DE653B0-F209-C441-84F9-A72667F02786}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,21 +44,9 @@
     <t xml:space="preserve">Potter </t>
   </si>
   <si>
-    <t xml:space="preserve">Comput er Science </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Graduat e </t>
-  </si>
-  <si>
     <t xml:space="preserve">Main Campus </t>
   </si>
   <si>
-    <t xml:space="preserve">hpotter 1@gsu. edu </t>
-  </si>
-  <si>
-    <t xml:space="preserve">College of Arts and Science s </t>
-  </si>
-  <si>
     <t xml:space="preserve">002142 876 </t>
   </si>
   <si>
@@ -71,9 +59,6 @@
     <t xml:space="preserve">Biology </t>
   </si>
   <si>
-    <t xml:space="preserve">astark1 @gsu.e du </t>
-  </si>
-  <si>
     <t xml:space="preserve">School of public health </t>
   </si>
   <si>
@@ -111,13 +96,28 @@
   </si>
   <si>
     <t>Email_Id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Computer Science </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Graduate </t>
+  </si>
+  <si>
+    <t xml:space="preserve">astark1@gsu.edu </t>
+  </si>
+  <si>
+    <t xml:space="preserve">hpotter1@gsu.edu </t>
+  </si>
+  <si>
+    <t>College of Arts and Sciences</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -137,6 +137,14 @@
       <color theme="1"/>
       <name val="TimesNewRomanPSMT"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -155,15 +163,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="12">
@@ -994,8 +1005,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{94FE30B2-D3C3-D74E-8868-1F67DB10D24E}" name="Table2" displayName="Table2" ref="A1:J4" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J4" xr:uid="{E9EE4E6E-0D38-1A44-AC02-31A9B91C86F7}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{94FE30B2-D3C3-D74E-8868-1F67DB10D24E}" name="Table2" displayName="Table2" ref="A1:J3" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J3" xr:uid="{E9EE4E6E-0D38-1A44-AC02-31A9B91C86F7}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{8DF3015A-6A83-DF4E-A26C-A4606800B430}" name="Panther_Id" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{9359BE57-650B-0442-B117-F587D9AA8EFA}" name="First_Name" dataDxfId="8"/>
@@ -1312,56 +1323,55 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="33.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.19921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.19921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.69921875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="21">
       <c r="A1" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>21</v>
-      </c>
     </row>
-    <row r="2" spans="1:10" ht="20">
+    <row r="2" spans="1:10" ht="21">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1372,60 +1382,60 @@
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="G2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>6</v>
+        <v>12</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="J2" s="2">
         <v>2020</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="20">
+    <row r="3" spans="1:10" ht="21">
       <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="J3" s="2">
         <v>2020</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="20">
+    <row r="4" spans="1:10" ht="21">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -1438,10 +1448,14 @@
       <c r="J4" s="2"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H3" r:id="rId1" xr:uid="{E86BA822-A343-48CD-8264-17737D1E95B2}"/>
+    <hyperlink ref="H2" r:id="rId2" xr:uid="{DB6C0B25-A743-4834-9D56-0454E08CEBBD}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId3"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>